<commit_message>
New docu on management
</commit_message>
<xml_diff>
--- a/openETCS ArchitectureAndDesign/Management/Working Groups_WP 3.xlsx
+++ b/openETCS ArchitectureAndDesign/Management/Working Groups_WP 3.xlsx
@@ -14,32 +14,17 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="42">
   <si>
     <t>Group 1</t>
   </si>
   <si>
-    <t>Fausto Cochetti</t>
-  </si>
-  <si>
-    <t>Christian Giraud</t>
-  </si>
-  <si>
-    <t>Veronique Gontier</t>
-  </si>
-  <si>
     <t>Group 2</t>
   </si>
   <si>
-    <t>Benjamin Beichler</t>
-  </si>
-  <si>
     <t>DB Group</t>
   </si>
   <si>
-    <t>Fraunhofer</t>
-  </si>
-  <si>
     <t>Data Dictionary</t>
   </si>
   <si>
@@ -49,21 +34,12 @@
     <t>Group 4</t>
   </si>
   <si>
-    <t>Peyman Farhangi</t>
-  </si>
-  <si>
     <t>Systerel</t>
   </si>
   <si>
-    <t>NS</t>
-  </si>
-  <si>
     <t>Speed and distance monitoring</t>
   </si>
   <si>
-    <t>Siemens</t>
-  </si>
-  <si>
     <t>Input Channel for the balis</t>
   </si>
   <si>
@@ -79,33 +55,18 @@
     <t>Data structure</t>
   </si>
   <si>
-    <t>TWT</t>
-  </si>
-  <si>
     <t>Train position and coordinate system</t>
   </si>
   <si>
     <t>Data Base</t>
   </si>
   <si>
-    <t>Jakob Gärtner</t>
-  </si>
-  <si>
     <t xml:space="preserve">Overall architecture leader </t>
   </si>
   <si>
     <t>API and Runtime system</t>
   </si>
   <si>
-    <t>Bend Hekele</t>
-  </si>
-  <si>
-    <t>David Mentre</t>
-  </si>
-  <si>
-    <t>Uwe Steinke</t>
-  </si>
-  <si>
     <t>SysMl General Support</t>
   </si>
   <si>
@@ -143,6 +104,42 @@
   </si>
   <si>
     <t>Christian Stahl, TWT</t>
+  </si>
+  <si>
+    <t>Uwe Steinke, Siemens</t>
+  </si>
+  <si>
+    <t>Bend Hekele, DB</t>
+  </si>
+  <si>
+    <t>Jakob Gärtner, DB (LEA)</t>
+  </si>
+  <si>
+    <t>David Mentre, Mitsubishi</t>
+  </si>
+  <si>
+    <t>Benjamin Beichler, UOR</t>
+  </si>
+  <si>
+    <t>Veronique Gontier, All4Tech</t>
+  </si>
+  <si>
+    <t>Christian Giraud, Alstom</t>
+  </si>
+  <si>
+    <t>Fausto Cochetti, Alstom</t>
+  </si>
+  <si>
+    <t>Alexander Stante, Fraunhofer</t>
+  </si>
+  <si>
+    <t>Peyman Farhangi, DB</t>
+  </si>
+  <si>
+    <t>Jan Welvaarts und Vincent Nuhaan, NS Team</t>
+  </si>
+  <si>
+    <t>SQS Team</t>
   </si>
 </sst>
 </file>
@@ -244,6 +241,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -253,9 +253,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -559,8 +556,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C4:L28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -570,109 +567,109 @@
     <col min="5" max="5" width="39.28515625" customWidth="1"/>
     <col min="6" max="6" width="32.85546875" customWidth="1"/>
     <col min="7" max="7" width="33.42578125" customWidth="1"/>
-    <col min="8" max="8" width="25.28515625" customWidth="1"/>
+    <col min="8" max="8" width="27.28515625" customWidth="1"/>
     <col min="9" max="9" width="24.42578125" customWidth="1"/>
-    <col min="10" max="10" width="38.85546875" customWidth="1"/>
+    <col min="10" max="10" width="43.42578125" customWidth="1"/>
     <col min="11" max="11" width="37.5703125" customWidth="1"/>
     <col min="12" max="12" width="23.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="4" spans="3:12" x14ac:dyDescent="0.25">
       <c r="G4" s="1" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="3:12" x14ac:dyDescent="0.25">
       <c r="G5" s="2" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
     </row>
     <row r="12" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
       <c r="E12" s="4" t="s">
-        <v>31</v>
+        <v>18</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>37</v>
+        <v>24</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="I12" s="4" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
       <c r="J12" s="4" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
       <c r="K12" s="4" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="L12" s="4"/>
     </row>
     <row r="13" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C13" s="4" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>34</v>
+        <v>21</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>30</v>
+        <v>17</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="G13" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H13" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="I13" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="I13" s="4" t="s">
-        <v>9</v>
-      </c>
       <c r="J13" s="4" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="K13" s="4" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="L13" s="4" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
     </row>
     <row r="14" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C14" s="2"/>
       <c r="D14" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E14" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="E14" s="2" t="s">
+      <c r="F14" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="F14" s="2" t="s">
-        <v>27</v>
-      </c>
       <c r="G14" s="2" t="s">
-        <v>1</v>
+        <v>37</v>
       </c>
       <c r="H14" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="I14" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="I14" s="2" t="s">
-        <v>12</v>
-      </c>
       <c r="J14" s="2" t="s">
-        <v>13</v>
+        <v>40</v>
       </c>
       <c r="K14" s="2" t="s">
-        <v>11</v>
+        <v>39</v>
       </c>
       <c r="L14" s="2" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
     </row>
     <row r="15" spans="3:12" x14ac:dyDescent="0.25">
@@ -680,17 +677,17 @@
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
       <c r="F15" s="2" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>2</v>
+        <v>36</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>7</v>
+        <v>38</v>
       </c>
       <c r="I15" s="2"/>
       <c r="J15" s="2" t="s">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="K15" s="2"/>
       <c r="L15" s="2"/>
@@ -700,16 +697,14 @@
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
       <c r="F16" s="2" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>3</v>
+        <v>35</v>
       </c>
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
-      <c r="J16" s="2" t="s">
-        <v>21</v>
-      </c>
+      <c r="J16" s="2"/>
       <c r="K16" s="2"/>
       <c r="L16" s="2"/>
     </row>
@@ -718,10 +713,10 @@
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
       <c r="F17" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>5</v>
+        <v>34</v>
       </c>
       <c r="H17" s="2"/>
       <c r="I17" s="2"/>
@@ -731,31 +726,31 @@
     </row>
     <row r="18" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C18" s="2"/>
-      <c r="D18" s="8"/>
-      <c r="E18" s="9"/>
-      <c r="F18" s="9"/>
-      <c r="G18" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="H18" s="9"/>
-      <c r="I18" s="9"/>
-      <c r="J18" s="9"/>
-      <c r="K18" s="9"/>
-      <c r="L18" s="10"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6"/>
+      <c r="G18" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="H18" s="6"/>
+      <c r="I18" s="6"/>
+      <c r="J18" s="6"/>
+      <c r="K18" s="6"/>
+      <c r="L18" s="7"/>
     </row>
     <row r="19" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C19" s="2"/>
-      <c r="D19" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="E19" s="6"/>
-      <c r="F19" s="6"/>
-      <c r="G19" s="6"/>
-      <c r="H19" s="6"/>
-      <c r="I19" s="6"/>
-      <c r="J19" s="6"/>
-      <c r="K19" s="6"/>
-      <c r="L19" s="7"/>
+      <c r="D19" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="E19" s="9"/>
+      <c r="F19" s="9"/>
+      <c r="G19" s="9"/>
+      <c r="H19" s="9"/>
+      <c r="I19" s="9"/>
+      <c r="J19" s="9"/>
+      <c r="K19" s="9"/>
+      <c r="L19" s="10"/>
     </row>
     <row r="20" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C20" s="3">
@@ -765,16 +760,16 @@
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
       <c r="G20" s="2" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="J20" s="2" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="K20" s="2"/>
       <c r="L20" s="2"/>
@@ -788,7 +783,7 @@
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
       <c r="H21" s="2" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="I21" s="2"/>
       <c r="J21" s="2"/>
@@ -804,7 +799,7 @@
       <c r="F22" s="2"/>
       <c r="G22" s="2"/>
       <c r="H22" s="2" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="I22" s="2"/>
       <c r="J22" s="2"/>
@@ -820,7 +815,7 @@
       <c r="F23" s="2"/>
       <c r="G23" s="2"/>
       <c r="H23" s="2" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="I23" s="2"/>
       <c r="J23" s="2"/>

</xml_diff>